<commit_message>
Updated all Infinity Functions
hanson-bas\misc\infinityFunction_Review
</commit_message>
<xml_diff>
--- a/misc/infinityFunction_Review.xlsx
+++ b/misc/infinityFunction_Review.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\coals01826\Desktop\Coding\hanson-bas\misc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{9F531A32-FFB9-4D51-AD42-93E3477A17AE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98194C34-B6D7-4491-B017-56DD2BD23DF4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="780" yWindow="780" windowWidth="21600" windowHeight="11385" xr2:uid="{CE91885B-EB52-4C98-81F8-BA09BC2838E4}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{CE91885B-EB52-4C98-81F8-BA09BC2838E4}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="29">
   <si>
     <t>boiler_test</t>
   </si>
@@ -96,20 +96,29 @@
     <t>10.1.13.71/pe/</t>
   </si>
   <si>
-    <t>???</t>
-  </si>
-  <si>
     <t>Good</t>
   </si>
   <si>
     <t>error on line 4 at column 1: Extra content at the end of the document</t>
+  </si>
+  <si>
+    <t>Full Address</t>
+  </si>
+  <si>
+    <t>error on line 8 at column 1: Extra content at the end of the document</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Good </t>
+  </si>
+  <si>
+    <t xml:space="preserve">% Good </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -118,10 +127,18 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="9"/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color rgb="FF000000"/>
-      <name val="Courier New"/>
-      <family val="3"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -141,15 +158,19 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -461,175 +482,314 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{19CF3B51-4B99-4D7B-9E44-3624160CD61C}">
-  <dimension ref="A1:C16"/>
+  <dimension ref="A1:G16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+      <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="63.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.140625" style="1"/>
+    <col min="2" max="2" width="13.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="27.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="63.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B1" t="s">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C1" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>22</v>
-      </c>
-      <c r="B2" t="s">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" s="1">
         <v>0</v>
       </c>
-      <c r="C2" t="s">
+      <c r="B2" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D2" s="1" t="str">
+        <f>CONCATENATE(B2,C2,".xml")</f>
+        <v>10.1.13.71/pe/boiler_test.xml</v>
+      </c>
+      <c r="E2" s="1" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>22</v>
-      </c>
-      <c r="B3" t="s">
+      <c r="F2" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="G2" s="1">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" s="1">
+        <v>1</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C3" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D3" s="1" t="str">
+        <f t="shared" ref="D3:D16" si="0">CONCATENATE(B3,C3,".xml")</f>
+        <v>10.1.13.71/pe/cx1_test.xml</v>
+      </c>
+      <c r="E3" s="1" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>22</v>
-      </c>
-      <c r="B4" t="s">
+      <c r="F3" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="G3" s="3">
+        <f>G2/(COUNT(A:A))</f>
+        <v>0.46666666666666667</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" s="1">
+        <v>2</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C4" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="1" t="s">
+      <c r="D4" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>10.1.13.71/pe/rtu1_test.xml</v>
+      </c>
+      <c r="E4" s="2" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>22</v>
-      </c>
-      <c r="B5" t="s">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" s="1">
         <v>3</v>
       </c>
-      <c r="C5" t="s">
+      <c r="B5" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D5" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>10.1.13.71/pe/rtu2_test.xml</v>
+      </c>
+      <c r="E5" s="1" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>22</v>
-      </c>
-      <c r="B6" t="s">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" s="1">
         <v>4</v>
       </c>
-      <c r="C6" t="s">
+      <c r="B6" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D6" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>10.1.13.71/pe/vav1.1_test.xml</v>
+      </c>
+      <c r="E6" s="1" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>22</v>
-      </c>
-      <c r="B7" t="s">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" s="1">
         <v>5</v>
       </c>
-      <c r="C7" t="s">
+      <c r="B7" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D7" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>10.1.13.71/pe/vav1.2_test.xml</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" s="1">
+        <v>6</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D8" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>10.1.13.71/pe/vav1.3_test.xml</v>
+      </c>
+      <c r="E8" s="1" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>22</v>
-      </c>
-      <c r="B8" t="s">
-        <v>6</v>
-      </c>
-      <c r="C8" t="s">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" s="1">
+        <v>7</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D9" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>10.1.13.71/pe/vav1.4_test.xml</v>
+      </c>
+      <c r="E9" s="1" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>22</v>
-      </c>
-      <c r="B9" t="s">
-        <v>7</v>
-      </c>
-      <c r="C9" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>22</v>
-      </c>
-      <c r="B10" t="s">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" s="1">
         <v>8</v>
       </c>
-      <c r="C10" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>22</v>
-      </c>
-      <c r="B11" t="s">
+      <c r="B10" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D10" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>10.1.13.71/pe/vav1.6_test.xml</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" s="1">
         <v>9</v>
       </c>
-      <c r="C11" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>22</v>
-      </c>
-      <c r="B12" t="s">
+      <c r="B11" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D11" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>10.1.13.71/pe/vav1.9_test.xml</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12" s="1">
         <v>10</v>
       </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>22</v>
-      </c>
-      <c r="B13" t="s">
+      <c r="B12" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D12" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>10.1.13.71/pe/vav1.10_test.xml</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13" s="1">
         <v>11</v>
       </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>22</v>
-      </c>
-      <c r="B14" t="s">
+      <c r="B13" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D13" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>10.1.13.71/pe/vav2.3_test.xml</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14" s="1">
         <v>12</v>
       </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>22</v>
-      </c>
-      <c r="B15" t="s">
+      <c r="B14" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D14" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>10.1.13.71/pe/vav2.6_test.xml</v>
+      </c>
+      <c r="E14" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A15" s="1">
         <v>13</v>
       </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>22</v>
-      </c>
-      <c r="B16" t="s">
+      <c r="B15" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D15" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>10.1.13.71/pe/vav2.8_test.xml</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A16" s="1">
         <v>14</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D16" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>10.1.13.71/pe/vav4.11_test.xml</v>
+      </c>
+      <c r="E16" s="2" t="s">
+        <v>18</v>
       </c>
     </row>
   </sheetData>

</xml_diff>